<commit_message>
Cambios en cuaderno de estudio
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado10/guion02/ESCALETA_MA_10_02_CO.xlsx
+++ b/fuentes/contenidos/grado10/guion02/ESCALETA_MA_10_02_CO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Documents\Aula Planeta Colombia\Repositorios\Matematicas\fuentes\contenidos\grado10\guion02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EdgarJosué\Documents\GitHub\Matematicas\fuentes\contenidos\grado10\guion02\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7650"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="3" r:id="rId1"/>
@@ -1090,6 +1090,36 @@
     <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1146,36 +1176,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1483,116 +1483,116 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="Q27" sqref="Q27:U27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.3984375" customWidth="1"/>
-    <col min="2" max="2" width="12.9296875" customWidth="1"/>
-    <col min="3" max="3" width="37.46484375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.33203125" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" customWidth="1"/>
-    <col min="7" max="7" width="17.73046875" customWidth="1"/>
-    <col min="17" max="17" width="5.9296875" style="35" customWidth="1"/>
-    <col min="18" max="18" width="4.46484375" style="35" customWidth="1"/>
-    <col min="19" max="19" width="33.46484375" style="35" customWidth="1"/>
-    <col min="20" max="20" width="52.33203125" style="35" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.28515625" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="17" max="17" width="6" style="35" customWidth="1"/>
+    <col min="18" max="18" width="4.42578125" style="35" customWidth="1"/>
+    <col min="19" max="19" width="33.42578125" style="35" customWidth="1"/>
+    <col min="20" max="20" width="52.28515625" style="35" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="14" style="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A1" s="65" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="65" t="s">
+      <c r="D1" s="75" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="67" t="s">
+      <c r="E1" s="77" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="72" t="s">
+      <c r="F1" s="82" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="63" t="s">
+      <c r="G1" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="74" t="s">
+      <c r="H1" s="84" t="s">
         <v>78</v>
       </c>
-      <c r="I1" s="76" t="s">
+      <c r="I1" s="86" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="78" t="s">
+      <c r="J1" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="80" t="s">
+      <c r="K1" s="90" t="s">
         <v>73</v>
       </c>
-      <c r="L1" s="63" t="s">
+      <c r="L1" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="84" t="s">
+      <c r="M1" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="84"/>
-      <c r="O1" s="85" t="s">
+      <c r="N1" s="65"/>
+      <c r="O1" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="P1" s="87" t="s">
+      <c r="P1" s="68" t="s">
         <v>79</v>
       </c>
-      <c r="Q1" s="89" t="s">
+      <c r="Q1" s="70" t="s">
         <v>65</v>
       </c>
-      <c r="R1" s="90" t="s">
+      <c r="R1" s="71" t="s">
         <v>66</v>
       </c>
-      <c r="S1" s="91" t="s">
+      <c r="S1" s="72" t="s">
         <v>67</v>
       </c>
-      <c r="T1" s="82" t="s">
+      <c r="T1" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="U1" s="83" t="s">
+      <c r="U1" s="64" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="66"/>
-      <c r="B2" s="68"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="79"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="64"/>
+    <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="76"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="87"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="74"/>
       <c r="M2" s="49" t="s">
         <v>70</v>
       </c>
       <c r="N2" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="O2" s="86"/>
-      <c r="P2" s="88"/>
-      <c r="Q2" s="89"/>
-      <c r="R2" s="90"/>
-      <c r="S2" s="91"/>
-      <c r="T2" s="82"/>
-      <c r="U2" s="83"/>
-    </row>
-    <row r="3" spans="1:21" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="O2" s="67"/>
+      <c r="P2" s="69"/>
+      <c r="Q2" s="70"/>
+      <c r="R2" s="71"/>
+      <c r="S2" s="72"/>
+      <c r="T2" s="63"/>
+      <c r="U2" s="64"/>
+    </row>
+    <row r="3" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>110</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>110</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>110</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>110</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>110</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>110</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>110</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>110</v>
       </c>
@@ -2048,7 +2048,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>110</v>
       </c>
@@ -2107,7 +2107,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>110</v>
       </c>
@@ -2164,7 +2164,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>110</v>
       </c>
@@ -2219,7 +2219,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>110</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>110</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>110</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>110</v>
       </c>
@@ -2449,7 +2449,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>110</v>
       </c>
@@ -2504,7 +2504,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>110</v>
       </c>
@@ -2559,7 +2559,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>110</v>
       </c>
@@ -2614,7 +2614,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>110</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>110</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>110</v>
       </c>
@@ -2789,7 +2789,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>110</v>
       </c>
@@ -2843,7 +2843,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>110</v>
       </c>
@@ -2897,7 +2897,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="26" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>110</v>
       </c>
@@ -2942,7 +2942,7 @@
       <c r="T26" s="62"/>
       <c r="U26" s="61"/>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>110</v>
       </c>
@@ -2997,7 +2997,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="28" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>110</v>
       </c>
@@ -3054,14 +3054,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="S1:S2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -3074,6 +3066,14 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:S2"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P3">
@@ -3125,27 +3125,27 @@
       <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.86328125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="34" style="1" customWidth="1"/>
-    <col min="5" max="5" width="34.86328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.59765625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="18" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.73046875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.59765625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" style="1" customWidth="1"/>
     <col min="12" max="12" width="17" style="1" customWidth="1"/>
-    <col min="13" max="13" width="11.3984375" style="1"/>
-    <col min="14" max="14" width="24.265625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="69.86328125" style="1" hidden="1" customWidth="1"/>
-    <col min="16" max="16384" width="11.3984375" style="1"/>
+    <col min="13" max="13" width="11.42578125" style="1"/>
+    <col min="14" max="14" width="24.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="69.85546875" style="1" hidden="1" customWidth="1"/>
+    <col min="16" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -3162,7 +3162,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -3186,7 +3186,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -3205,7 +3205,7 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -3224,7 +3224,7 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
@@ -3240,7 +3240,7 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
@@ -3257,7 +3257,7 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
@@ -3274,7 +3274,7 @@
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -3289,7 +3289,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -3304,7 +3304,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -3319,7 +3319,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -3334,7 +3334,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -3349,7 +3349,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -3364,7 +3364,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -3379,7 +3379,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -3394,7 +3394,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -3409,7 +3409,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="1" t="s">
@@ -3423,7 +3423,7 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="1" t="s">
@@ -3437,7 +3437,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="1" t="s">
@@ -3451,7 +3451,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="1" t="s">
@@ -3465,7 +3465,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -3480,7 +3480,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -3495,7 +3495,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -3510,7 +3510,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="24" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -3525,7 +3525,7 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -3540,7 +3540,7 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -3555,7 +3555,7 @@
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="27" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -3570,7 +3570,7 @@
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -3585,7 +3585,7 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="29" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -3600,7 +3600,7 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -3615,7 +3615,7 @@
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -3630,7 +3630,7 @@
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
     </row>
-    <row r="32" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="32" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -3645,7 +3645,7 @@
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
     </row>
-    <row r="33" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -3660,7 +3660,7 @@
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="34" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -3675,7 +3675,7 @@
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
     </row>
-    <row r="35" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="35" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -3690,7 +3690,7 @@
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
     </row>
-    <row r="36" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="36" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -3705,7 +3705,7 @@
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
     </row>
-    <row r="37" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="37" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -3720,7 +3720,7 @@
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
     </row>
-    <row r="38" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="38" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -3735,7 +3735,7 @@
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
     </row>
-    <row r="39" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="39" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -3750,7 +3750,7 @@
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
     </row>
-    <row r="40" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="40" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -3765,7 +3765,7 @@
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
     </row>
-    <row r="41" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="41" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -3780,7 +3780,7 @@
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
     </row>
-    <row r="42" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="42" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -3795,7 +3795,7 @@
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
     </row>
-    <row r="43" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="43" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -3810,7 +3810,7 @@
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
     </row>
-    <row r="44" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="44" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -3825,7 +3825,7 @@
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
     </row>
-    <row r="45" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="45" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -3840,7 +3840,7 @@
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
     </row>
-    <row r="46" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="46" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -3855,7 +3855,7 @@
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
     </row>
-    <row r="47" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="47" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -3870,7 +3870,7 @@
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
     </row>
-    <row r="48" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="48" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -3885,7 +3885,7 @@
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
     </row>
-    <row r="49" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="49" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -3897,7 +3897,7 @@
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
     </row>
-    <row r="50" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="50" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -3909,7 +3909,7 @@
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
     </row>
-    <row r="51" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="51" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -3922,7 +3922,7 @@
       <c r="K51" s="2"/>
       <c r="L51" s="2"/>
     </row>
-    <row r="52" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="52" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -3935,7 +3935,7 @@
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
     </row>
-    <row r="53" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="53" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -3948,7 +3948,7 @@
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
     </row>
-    <row r="54" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="54" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -3961,7 +3961,7 @@
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
     </row>
-    <row r="55" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="55" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
@@ -3974,7 +3974,7 @@
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
     </row>
-    <row r="56" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="56" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -3987,7 +3987,7 @@
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
     </row>
-    <row r="57" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="57" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
@@ -4000,7 +4000,7 @@
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
     </row>
-    <row r="58" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="58" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
@@ -4013,7 +4013,7 @@
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
     </row>
-    <row r="59" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="59" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -4026,7 +4026,7 @@
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
     </row>
-    <row r="60" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="60" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -4039,7 +4039,7 @@
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
     </row>
-    <row r="61" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="61" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
@@ -4052,7 +4052,7 @@
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
     </row>
-    <row r="62" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="62" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
@@ -4065,7 +4065,7 @@
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
     </row>
-    <row r="63" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="63" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
@@ -4078,7 +4078,7 @@
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
     </row>
-    <row r="64" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="64" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
@@ -4091,7 +4091,7 @@
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
     </row>
-    <row r="65" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
@@ -4104,7 +4104,7 @@
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
     </row>
-    <row r="66" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
@@ -4117,7 +4117,7 @@
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
     </row>
-    <row r="67" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
@@ -4130,7 +4130,7 @@
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
     </row>
-    <row r="68" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
@@ -4143,7 +4143,7 @@
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
     </row>
-    <row r="69" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
@@ -4156,7 +4156,7 @@
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
     </row>
-    <row r="70" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
@@ -4169,7 +4169,7 @@
       <c r="K70" s="2"/>
       <c r="L70" s="2"/>
     </row>
-    <row r="71" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -4183,7 +4183,7 @@
       <c r="K71" s="2"/>
       <c r="L71" s="2"/>
     </row>
-    <row r="72" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -4197,7 +4197,7 @@
       <c r="K72" s="2"/>
       <c r="L72" s="2"/>
     </row>
-    <row r="73" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -4211,7 +4211,7 @@
       <c r="K73" s="2"/>
       <c r="L73" s="2"/>
     </row>
-    <row r="74" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -4225,7 +4225,7 @@
       <c r="K74" s="2"/>
       <c r="L74" s="2"/>
     </row>
-    <row r="75" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -4239,7 +4239,7 @@
       <c r="K75" s="2"/>
       <c r="L75" s="2"/>
     </row>
-    <row r="76" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -4253,7 +4253,7 @@
       <c r="K76" s="2"/>
       <c r="L76" s="2"/>
     </row>
-    <row r="77" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -4267,7 +4267,7 @@
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
     </row>
-    <row r="78" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -4281,7 +4281,7 @@
       <c r="K78" s="2"/>
       <c r="L78" s="2"/>
     </row>
-    <row r="79" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -4295,7 +4295,7 @@
       <c r="K79" s="2"/>
       <c r="L79" s="2"/>
     </row>
-    <row r="80" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -4309,7 +4309,7 @@
       <c r="K80" s="2"/>
       <c r="L80" s="2"/>
     </row>
-    <row r="81" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -4323,7 +4323,7 @@
       <c r="K81" s="2"/>
       <c r="L81" s="2"/>
     </row>
-    <row r="82" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -4337,7 +4337,7 @@
       <c r="K82" s="2"/>
       <c r="L82" s="2"/>
     </row>
-    <row r="83" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -4351,7 +4351,7 @@
       <c r="K83" s="2"/>
       <c r="L83" s="2"/>
     </row>
-    <row r="84" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -4365,7 +4365,7 @@
       <c r="K84" s="2"/>
       <c r="L84" s="2"/>
     </row>
-    <row r="85" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -4379,7 +4379,7 @@
       <c r="K85" s="2"/>
       <c r="L85" s="2"/>
     </row>
-    <row r="86" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -4393,7 +4393,7 @@
       <c r="K86" s="2"/>
       <c r="L86" s="2"/>
     </row>
-    <row r="87" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -4407,7 +4407,7 @@
       <c r="K87" s="2"/>
       <c r="L87" s="2"/>
     </row>
-    <row r="88" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -4421,7 +4421,7 @@
       <c r="K88" s="2"/>
       <c r="L88" s="2"/>
     </row>
-    <row r="89" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -4435,7 +4435,7 @@
       <c r="K89" s="2"/>
       <c r="L89" s="2"/>
     </row>
-    <row r="90" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -4449,7 +4449,7 @@
       <c r="K90" s="2"/>
       <c r="L90" s="2"/>
     </row>
-    <row r="91" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -4463,7 +4463,7 @@
       <c r="K91" s="2"/>
       <c r="L91" s="2"/>
     </row>
-    <row r="92" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -4477,7 +4477,7 @@
       <c r="K92" s="2"/>
       <c r="L92" s="2"/>
     </row>
-    <row r="93" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -4491,7 +4491,7 @@
       <c r="K93" s="2"/>
       <c r="L93" s="2"/>
     </row>
-    <row r="94" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="94" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -4505,7 +4505,7 @@
       <c r="K94" s="2"/>
       <c r="L94" s="2"/>
     </row>
-    <row r="95" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -4519,7 +4519,7 @@
       <c r="K95" s="2"/>
       <c r="L95" s="2"/>
     </row>
-    <row r="96" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="96" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -4533,7 +4533,7 @@
       <c r="K96" s="2"/>
       <c r="L96" s="2"/>
     </row>
-    <row r="97" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -4547,7 +4547,7 @@
       <c r="K97" s="2"/>
       <c r="L97" s="2"/>
     </row>
-    <row r="98" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -4561,7 +4561,7 @@
       <c r="K98" s="2"/>
       <c r="L98" s="2"/>
     </row>
-    <row r="99" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="99" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -4575,7 +4575,7 @@
       <c r="K99" s="2"/>
       <c r="L99" s="2"/>
     </row>
-    <row r="100" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="100" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -4589,7 +4589,7 @@
       <c r="K100" s="2"/>
       <c r="L100" s="2"/>
     </row>
-    <row r="101" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="101" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -4603,7 +4603,7 @@
       <c r="K101" s="2"/>
       <c r="L101" s="2"/>
     </row>
-    <row r="102" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="102" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -4617,7 +4617,7 @@
       <c r="K102" s="2"/>
       <c r="L102" s="2"/>
     </row>
-    <row r="103" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="103" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -4631,7 +4631,7 @@
       <c r="K103" s="2"/>
       <c r="L103" s="2"/>
     </row>
-    <row r="104" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="104" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -4645,7 +4645,7 @@
       <c r="K104" s="2"/>
       <c r="L104" s="2"/>
     </row>
-    <row r="105" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="105" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -4659,7 +4659,7 @@
       <c r="K105" s="2"/>
       <c r="L105" s="2"/>
     </row>
-    <row r="106" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="106" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -4673,7 +4673,7 @@
       <c r="K106" s="2"/>
       <c r="L106" s="2"/>
     </row>
-    <row r="107" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="107" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -4687,7 +4687,7 @@
       <c r="K107" s="2"/>
       <c r="L107" s="2"/>
     </row>
-    <row r="108" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="108" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -4701,7 +4701,7 @@
       <c r="K108" s="2"/>
       <c r="L108" s="2"/>
     </row>
-    <row r="109" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="109" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -4715,7 +4715,7 @@
       <c r="K109" s="2"/>
       <c r="L109" s="2"/>
     </row>
-    <row r="110" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="110" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -4729,7 +4729,7 @@
       <c r="K110" s="2"/>
       <c r="L110" s="2"/>
     </row>
-    <row r="111" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="111" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -4743,7 +4743,7 @@
       <c r="K111" s="2"/>
       <c r="L111" s="2"/>
     </row>
-    <row r="112" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="112" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -4757,7 +4757,7 @@
       <c r="K112" s="2"/>
       <c r="L112" s="2"/>
     </row>
-    <row r="113" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="113" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -4771,7 +4771,7 @@
       <c r="K113" s="2"/>
       <c r="L113" s="2"/>
     </row>
-    <row r="114" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="114" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -4785,7 +4785,7 @@
       <c r="K114" s="2"/>
       <c r="L114" s="2"/>
     </row>
-    <row r="115" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="115" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -4799,7 +4799,7 @@
       <c r="K115" s="2"/>
       <c r="L115" s="2"/>
     </row>
-    <row r="116" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="116" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -4813,7 +4813,7 @@
       <c r="K116" s="2"/>
       <c r="L116" s="2"/>
     </row>
-    <row r="117" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="117" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -4827,7 +4827,7 @@
       <c r="K117" s="2"/>
       <c r="L117" s="2"/>
     </row>
-    <row r="118" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="118" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -4841,7 +4841,7 @@
       <c r="K118" s="2"/>
       <c r="L118" s="2"/>
     </row>
-    <row r="119" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="119" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -4855,7 +4855,7 @@
       <c r="K119" s="2"/>
       <c r="L119" s="2"/>
     </row>
-    <row r="120" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="120" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -4869,7 +4869,7 @@
       <c r="K120" s="2"/>
       <c r="L120" s="2"/>
     </row>
-    <row r="121" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="121" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="2"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
@@ -4883,7 +4883,7 @@
       <c r="K121" s="2"/>
       <c r="L121" s="2"/>
     </row>
-    <row r="122" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="122" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -4897,7 +4897,7 @@
       <c r="K122" s="2"/>
       <c r="L122" s="2"/>
     </row>
-    <row r="123" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="123" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -4911,7 +4911,7 @@
       <c r="K123" s="2"/>
       <c r="L123" s="2"/>
     </row>
-    <row r="124" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="124" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -4925,7 +4925,7 @@
       <c r="K124" s="2"/>
       <c r="L124" s="2"/>
     </row>
-    <row r="125" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="125" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
@@ -4939,7 +4939,7 @@
       <c r="K125" s="2"/>
       <c r="L125" s="2"/>
     </row>
-    <row r="126" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="126" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -4953,7 +4953,7 @@
       <c r="K126" s="2"/>
       <c r="L126" s="2"/>
     </row>
-    <row r="127" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="127" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -4967,7 +4967,7 @@
       <c r="K127" s="2"/>
       <c r="L127" s="2"/>
     </row>
-    <row r="128" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="128" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -4981,7 +4981,7 @@
       <c r="K128" s="2"/>
       <c r="L128" s="2"/>
     </row>
-    <row r="129" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="129" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="2"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
@@ -4995,7 +4995,7 @@
       <c r="K129" s="2"/>
       <c r="L129" s="2"/>
     </row>
-    <row r="130" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="130" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130" s="2"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -5009,7 +5009,7 @@
       <c r="K130" s="2"/>
       <c r="L130" s="2"/>
     </row>
-    <row r="131" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="131" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -5023,7 +5023,7 @@
       <c r="K131" s="2"/>
       <c r="L131" s="2"/>
     </row>
-    <row r="132" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="132" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -5037,7 +5037,7 @@
       <c r="K132" s="2"/>
       <c r="L132" s="2"/>
     </row>
-    <row r="133" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="133" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A133" s="2"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>

</xml_diff>

<commit_message>
Correcciones solicitadas por Lizzie
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado10/guion02/ESCALETA_MA_10_02_CO.xlsx
+++ b/fuentes/contenidos/grado10/guion02/ESCALETA_MA_10_02_CO.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="3" r:id="rId1"/>
@@ -930,7 +930,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1003,26 +1003,17 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1061,12 +1052,6 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1090,6 +1075,63 @@
     <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1120,62 +1162,54 @@
     <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1483,8 +1517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27:U27"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1494,103 +1528,103 @@
     <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39.28515625" customWidth="1"/>
     <col min="5" max="5" width="20.28515625" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" customWidth="1"/>
-    <col min="17" max="17" width="6" style="35" customWidth="1"/>
-    <col min="18" max="18" width="4.42578125" style="35" customWidth="1"/>
-    <col min="19" max="19" width="33.42578125" style="35" customWidth="1"/>
-    <col min="20" max="20" width="52.28515625" style="35" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14" style="35" customWidth="1"/>
+    <col min="7" max="7" width="53.5703125" customWidth="1"/>
+    <col min="17" max="17" width="6" style="32" customWidth="1"/>
+    <col min="18" max="18" width="4.42578125" style="32" customWidth="1"/>
+    <col min="19" max="19" width="33.42578125" style="32" customWidth="1"/>
+    <col min="20" max="20" width="52.28515625" style="32" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14" style="32" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="77" t="s">
+      <c r="B1" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="79" t="s">
+      <c r="C1" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="75" t="s">
+      <c r="D1" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="77" t="s">
+      <c r="E1" s="62" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="82" t="s">
+      <c r="F1" s="67" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="73" t="s">
+      <c r="G1" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="84" t="s">
+      <c r="H1" s="69" t="s">
         <v>78</v>
       </c>
-      <c r="I1" s="86" t="s">
+      <c r="I1" s="71" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="88" t="s">
+      <c r="J1" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="90" t="s">
+      <c r="K1" s="75" t="s">
         <v>73</v>
       </c>
-      <c r="L1" s="73" t="s">
+      <c r="L1" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="65" t="s">
+      <c r="M1" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="65"/>
-      <c r="O1" s="66" t="s">
+      <c r="N1" s="79"/>
+      <c r="O1" s="80" t="s">
         <v>74</v>
       </c>
-      <c r="P1" s="68" t="s">
+      <c r="P1" s="82" t="s">
         <v>79</v>
       </c>
-      <c r="Q1" s="70" t="s">
+      <c r="Q1" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="R1" s="71" t="s">
+      <c r="R1" s="85" t="s">
         <v>66</v>
       </c>
-      <c r="S1" s="72" t="s">
+      <c r="S1" s="86" t="s">
         <v>67</v>
       </c>
-      <c r="T1" s="63" t="s">
+      <c r="T1" s="77" t="s">
         <v>68</v>
       </c>
-      <c r="U1" s="64" t="s">
+      <c r="U1" s="78" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="76"/>
-      <c r="B2" s="78"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="87"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="91"/>
-      <c r="L2" s="74"/>
-      <c r="M2" s="49" t="s">
+      <c r="A2" s="61"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="N2" s="49" t="s">
+      <c r="N2" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="O2" s="67"/>
-      <c r="P2" s="69"/>
-      <c r="Q2" s="70"/>
-      <c r="R2" s="71"/>
-      <c r="S2" s="72"/>
-      <c r="T2" s="63"/>
-      <c r="U2" s="64"/>
+      <c r="O2" s="81"/>
+      <c r="P2" s="83"/>
+      <c r="Q2" s="84"/>
+      <c r="R2" s="85"/>
+      <c r="S2" s="86"/>
+      <c r="T2" s="77"/>
+      <c r="U2" s="78"/>
     </row>
     <row r="3" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -1602,50 +1636,50 @@
       <c r="C3" t="s">
         <v>180</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="E3" s="37"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="43" t="s">
+      <c r="E3" s="34"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="87" t="s">
         <v>111</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="88">
         <v>1</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="89" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="29" t="s">
+      <c r="J3" s="90" t="s">
         <v>112</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="89" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="13"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="32" t="s">
+      <c r="M3" s="91"/>
+      <c r="N3" s="92"/>
+      <c r="O3" s="93" t="s">
         <v>113</v>
       </c>
-      <c r="P3" s="48" t="s">
+      <c r="P3" s="94" t="s">
         <v>114</v>
       </c>
-      <c r="Q3" s="50" t="s">
+      <c r="Q3" s="45" t="s">
         <v>115</v>
       </c>
-      <c r="R3" s="51" t="s">
+      <c r="R3" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="S3" s="50" t="s">
+      <c r="S3" s="45" t="s">
         <v>116</v>
       </c>
-      <c r="T3" s="52" t="s">
+      <c r="T3" s="47" t="s">
         <v>117</v>
       </c>
-      <c r="U3" s="51" t="s">
+      <c r="U3" s="46" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1659,12 +1693,12 @@
       <c r="C4" t="s">
         <v>180</v>
       </c>
-      <c r="D4" s="36" t="s">
+      <c r="D4" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="E4" s="37"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="44" t="s">
+      <c r="E4" s="34"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="41" t="s">
         <v>119</v>
       </c>
       <c r="H4" s="5">
@@ -1686,25 +1720,25 @@
       <c r="N4" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="O4" s="33" t="s">
+      <c r="O4" s="30" t="s">
         <v>157</v>
       </c>
       <c r="P4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Q4" s="53">
+      <c r="Q4" s="48">
         <v>6</v>
       </c>
-      <c r="R4" s="54" t="s">
+      <c r="R4" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="S4" s="53" t="s">
+      <c r="S4" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="T4" s="55" t="s">
+      <c r="T4" s="50" t="s">
         <v>164</v>
       </c>
-      <c r="U4" s="54" t="s">
+      <c r="U4" s="49" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1718,12 +1752,12 @@
       <c r="C5" t="s">
         <v>180</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="E5" s="37"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="43" t="s">
+      <c r="E5" s="34"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="40" t="s">
         <v>122</v>
       </c>
       <c r="H5" s="5">
@@ -1732,7 +1766,7 @@
       <c r="I5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="30" t="s">
+      <c r="J5" s="28" t="s">
         <v>121</v>
       </c>
       <c r="K5" s="4" t="s">
@@ -1745,25 +1779,25 @@
       <c r="N5" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="O5" s="33" t="s">
+      <c r="O5" s="30" t="s">
         <v>158</v>
       </c>
       <c r="P5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Q5" s="53">
+      <c r="Q5" s="48">
         <v>6</v>
       </c>
-      <c r="R5" s="54" t="s">
+      <c r="R5" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="S5" s="53" t="s">
+      <c r="S5" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="T5" s="55" t="s">
+      <c r="T5" s="50" t="s">
         <v>91</v>
       </c>
-      <c r="U5" s="54" t="s">
+      <c r="U5" s="49" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1777,12 +1811,12 @@
       <c r="C6" t="s">
         <v>180</v>
       </c>
-      <c r="D6" s="36" t="s">
+      <c r="D6" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="E6" s="37"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="43" t="s">
+      <c r="E6" s="34"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="40" t="s">
         <v>123</v>
       </c>
       <c r="H6" s="5">
@@ -1791,7 +1825,7 @@
       <c r="I6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="30" t="s">
+      <c r="J6" s="28" t="s">
         <v>155</v>
       </c>
       <c r="K6" s="4" t="s">
@@ -1802,23 +1836,23 @@
       </c>
       <c r="M6" s="13"/>
       <c r="N6" s="14"/>
-      <c r="O6" s="33"/>
+      <c r="O6" s="30"/>
       <c r="P6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Q6" s="53">
+      <c r="Q6" s="48">
         <v>6</v>
       </c>
-      <c r="R6" s="54" t="s">
+      <c r="R6" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="S6" s="53" t="s">
+      <c r="S6" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="T6" s="55" t="s">
+      <c r="T6" s="50" t="s">
         <v>167</v>
       </c>
-      <c r="U6" s="54" t="s">
+      <c r="U6" s="49" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1832,12 +1866,12 @@
       <c r="C7" t="s">
         <v>180</v>
       </c>
-      <c r="D7" s="36" t="s">
+      <c r="D7" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="E7" s="37"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="43" t="s">
+      <c r="E7" s="34"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="40" t="s">
         <v>124</v>
       </c>
       <c r="H7" s="5">
@@ -1846,7 +1880,7 @@
       <c r="I7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="30" t="s">
+      <c r="J7" s="28" t="s">
         <v>156</v>
       </c>
       <c r="K7" s="4" t="s">
@@ -1859,25 +1893,25 @@
       <c r="N7" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="O7" s="33" t="s">
+      <c r="O7" s="30" t="s">
         <v>171</v>
       </c>
       <c r="P7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Q7" s="53">
+      <c r="Q7" s="48">
         <v>6</v>
       </c>
-      <c r="R7" s="54" t="s">
+      <c r="R7" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="S7" s="53" t="s">
+      <c r="S7" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="T7" s="55" t="s">
+      <c r="T7" s="50" t="s">
         <v>97</v>
       </c>
-      <c r="U7" s="54" t="s">
+      <c r="U7" s="49" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1891,14 +1925,14 @@
       <c r="C8" t="s">
         <v>180</v>
       </c>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="33" t="s">
         <v>125</v>
       </c>
       <c r="E8" s="22" t="s">
         <v>168</v>
       </c>
-      <c r="F8" s="40"/>
-      <c r="G8" s="28" t="s">
+      <c r="F8" s="37"/>
+      <c r="G8" s="27" t="s">
         <v>105</v>
       </c>
       <c r="H8" s="5">
@@ -1922,19 +1956,19 @@
       <c r="P8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Q8" s="53">
+      <c r="Q8" s="48">
         <v>9</v>
       </c>
-      <c r="R8" s="54" t="s">
+      <c r="R8" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="S8" s="53" t="s">
+      <c r="S8" s="48" t="s">
         <v>126</v>
       </c>
-      <c r="T8" s="56" t="s">
+      <c r="T8" s="51" t="s">
         <v>105</v>
       </c>
-      <c r="U8" s="54" t="s">
+      <c r="U8" s="49" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1952,8 +1986,8 @@
         <v>100</v>
       </c>
       <c r="E9" s="22"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="28" t="s">
+      <c r="F9" s="38"/>
+      <c r="G9" s="27" t="s">
         <v>132</v>
       </c>
       <c r="H9" s="5">
@@ -1962,7 +1996,7 @@
       <c r="I9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="45" t="s">
+      <c r="J9" s="42" t="s">
         <v>140</v>
       </c>
       <c r="K9" s="4" t="s">
@@ -1977,19 +2011,19 @@
       <c r="P9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Q9" s="53">
+      <c r="Q9" s="48">
         <v>9</v>
       </c>
-      <c r="R9" s="54" t="s">
+      <c r="R9" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="S9" s="53" t="s">
+      <c r="S9" s="48" t="s">
         <v>126</v>
       </c>
-      <c r="T9" s="56" t="s">
+      <c r="T9" s="51" t="s">
         <v>132</v>
       </c>
-      <c r="U9" s="54" t="s">
+      <c r="U9" s="49" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2007,8 +2041,8 @@
         <v>100</v>
       </c>
       <c r="E10" s="19"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="28" t="s">
+      <c r="F10" s="37"/>
+      <c r="G10" s="27" t="s">
         <v>172</v>
       </c>
       <c r="H10" s="5">
@@ -2032,19 +2066,19 @@
       <c r="P10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Q10" s="53">
+      <c r="Q10" s="48">
         <v>9</v>
       </c>
-      <c r="R10" s="54" t="s">
+      <c r="R10" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="S10" s="53" t="s">
+      <c r="S10" s="48" t="s">
         <v>126</v>
       </c>
-      <c r="T10" s="56" t="s">
+      <c r="T10" s="51" t="s">
         <v>127</v>
       </c>
-      <c r="U10" s="54" t="s">
+      <c r="U10" s="49" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2062,8 +2096,8 @@
         <v>100</v>
       </c>
       <c r="E11" s="19"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="28" t="s">
+      <c r="F11" s="37"/>
+      <c r="G11" s="27" t="s">
         <v>133</v>
       </c>
       <c r="H11" s="5">
@@ -2091,19 +2125,19 @@
       <c r="P11" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="53">
+      <c r="Q11" s="48">
         <v>6</v>
       </c>
-      <c r="R11" s="54" t="s">
+      <c r="R11" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="S11" s="53" t="s">
+      <c r="S11" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="T11" s="55" t="s">
+      <c r="T11" s="50" t="s">
         <v>165</v>
       </c>
-      <c r="U11" s="54" t="s">
+      <c r="U11" s="49" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2123,8 +2157,8 @@
       <c r="E12" s="22" t="s">
         <v>168</v>
       </c>
-      <c r="F12" s="34"/>
-      <c r="G12" s="28" t="s">
+      <c r="F12" s="31"/>
+      <c r="G12" s="27" t="s">
         <v>106</v>
       </c>
       <c r="H12" s="5">
@@ -2142,25 +2176,25 @@
       <c r="L12" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="M12" s="31"/>
-      <c r="N12" s="31"/>
-      <c r="O12" s="34"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="31"/>
       <c r="P12" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Q12" s="53">
+      <c r="Q12" s="48">
         <v>9</v>
       </c>
-      <c r="R12" s="54" t="s">
+      <c r="R12" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="S12" s="53" t="s">
+      <c r="S12" s="48" t="s">
         <v>126</v>
       </c>
-      <c r="T12" s="56" t="s">
+      <c r="T12" s="51" t="s">
         <v>106</v>
       </c>
-      <c r="U12" s="54" t="s">
+      <c r="U12" s="49" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2178,44 +2212,44 @@
         <v>169</v>
       </c>
       <c r="E13" s="22"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="28" t="s">
+      <c r="F13" s="38"/>
+      <c r="G13" s="95" t="s">
         <v>130</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13" s="88">
         <v>11</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="I13" s="89" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="20" t="s">
+      <c r="J13" s="96" t="s">
         <v>144</v>
       </c>
-      <c r="K13" s="9" t="s">
+      <c r="K13" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="L13" s="12" t="s">
+      <c r="L13" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="M13" s="26"/>
-      <c r="N13" s="26"/>
-      <c r="O13" s="23"/>
-      <c r="P13" s="7" t="s">
+      <c r="M13" s="98"/>
+      <c r="N13" s="98"/>
+      <c r="O13" s="95"/>
+      <c r="P13" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="Q13" s="53">
+      <c r="Q13" s="48">
         <v>9</v>
       </c>
-      <c r="R13" s="54" t="s">
+      <c r="R13" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="S13" s="53" t="s">
+      <c r="S13" s="48" t="s">
         <v>126</v>
       </c>
-      <c r="T13" s="56" t="s">
+      <c r="T13" s="51" t="s">
         <v>130</v>
       </c>
-      <c r="U13" s="54" t="s">
+      <c r="U13" s="49" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2233,48 +2267,48 @@
         <v>169</v>
       </c>
       <c r="E14" s="22"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="28" t="s">
+      <c r="F14" s="38"/>
+      <c r="G14" s="95" t="s">
         <v>173</v>
       </c>
-      <c r="H14" s="5">
+      <c r="H14" s="88">
         <v>12</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="I14" s="89" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="20" t="s">
+      <c r="J14" s="96" t="s">
         <v>145</v>
       </c>
-      <c r="K14" s="9" t="s">
+      <c r="K14" s="97" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="12" t="s">
+      <c r="L14" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="M14" s="25"/>
-      <c r="N14" s="15" t="s">
+      <c r="M14" s="87"/>
+      <c r="N14" s="91" t="s">
         <v>33</v>
       </c>
-      <c r="O14" s="23" t="s">
+      <c r="O14" s="95" t="s">
         <v>161</v>
       </c>
-      <c r="P14" s="7" t="s">
+      <c r="P14" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="Q14" s="53">
+      <c r="Q14" s="48">
         <v>6</v>
       </c>
-      <c r="R14" s="54" t="s">
+      <c r="R14" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="S14" s="53" t="s">
+      <c r="S14" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="T14" s="55" t="s">
+      <c r="T14" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="U14" s="54" t="s">
+      <c r="U14" s="49" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2292,44 +2326,44 @@
         <v>169</v>
       </c>
       <c r="E15" s="22"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="28" t="s">
+      <c r="F15" s="38"/>
+      <c r="G15" s="95" t="s">
         <v>131</v>
       </c>
-      <c r="H15" s="5">
+      <c r="H15" s="88">
         <v>13</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="I15" s="89" t="s">
         <v>19</v>
       </c>
-      <c r="J15" s="45" t="s">
+      <c r="J15" s="100" t="s">
         <v>146</v>
       </c>
-      <c r="K15" s="9" t="s">
+      <c r="K15" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="L15" s="12" t="s">
+      <c r="L15" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="23"/>
-      <c r="P15" s="7" t="s">
+      <c r="M15" s="91"/>
+      <c r="N15" s="91"/>
+      <c r="O15" s="95"/>
+      <c r="P15" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="Q15" s="53">
+      <c r="Q15" s="48">
         <v>9</v>
       </c>
-      <c r="R15" s="54" t="s">
+      <c r="R15" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="S15" s="53" t="s">
+      <c r="S15" s="48" t="s">
         <v>126</v>
       </c>
-      <c r="T15" s="56" t="s">
+      <c r="T15" s="51" t="s">
         <v>131</v>
       </c>
-      <c r="U15" s="54" t="s">
+      <c r="U15" s="49" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2349,8 +2383,8 @@
       <c r="E16" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="F16" s="41"/>
-      <c r="G16" s="28" t="s">
+      <c r="F16" s="38"/>
+      <c r="G16" s="27" t="s">
         <v>107</v>
       </c>
       <c r="H16" s="5">
@@ -2374,19 +2408,19 @@
       <c r="P16" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Q16" s="53">
+      <c r="Q16" s="48">
         <v>9</v>
       </c>
-      <c r="R16" s="54" t="s">
+      <c r="R16" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="S16" s="53" t="s">
+      <c r="S16" s="48" t="s">
         <v>126</v>
       </c>
-      <c r="T16" s="56" t="s">
+      <c r="T16" s="51" t="s">
         <v>107</v>
       </c>
-      <c r="U16" s="54" t="s">
+      <c r="U16" s="49" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2404,48 +2438,48 @@
         <v>178</v>
       </c>
       <c r="E17" s="22"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="28" t="s">
+      <c r="F17" s="38"/>
+      <c r="G17" s="95" t="s">
         <v>135</v>
       </c>
-      <c r="H17" s="5">
+      <c r="H17" s="88">
         <v>15</v>
       </c>
-      <c r="I17" s="3" t="s">
+      <c r="I17" s="89" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="20" t="s">
+      <c r="J17" s="96" t="s">
         <v>174</v>
       </c>
-      <c r="K17" s="4" t="s">
+      <c r="K17" s="89" t="s">
         <v>20</v>
       </c>
-      <c r="L17" s="12" t="s">
+      <c r="L17" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15" t="s">
+      <c r="M17" s="91"/>
+      <c r="N17" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="O17" s="23" t="s">
+      <c r="O17" s="95" t="s">
         <v>162</v>
       </c>
-      <c r="P17" s="7" t="s">
+      <c r="P17" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="Q17" s="53">
+      <c r="Q17" s="48">
         <v>6</v>
       </c>
-      <c r="R17" s="54" t="s">
+      <c r="R17" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="S17" s="53" t="s">
+      <c r="S17" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="T17" s="55" t="s">
+      <c r="T17" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="U17" s="54" t="s">
+      <c r="U17" s="49" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2463,8 +2497,8 @@
         <v>178</v>
       </c>
       <c r="E18" s="19"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="28" t="s">
+      <c r="F18" s="37"/>
+      <c r="G18" s="27" t="s">
         <v>101</v>
       </c>
       <c r="H18" s="5">
@@ -2488,19 +2522,19 @@
       <c r="P18" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Q18" s="53">
+      <c r="Q18" s="48">
         <v>9</v>
       </c>
-      <c r="R18" s="54" t="s">
+      <c r="R18" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="S18" s="53" t="s">
+      <c r="S18" s="48" t="s">
         <v>126</v>
       </c>
-      <c r="T18" s="56" t="s">
+      <c r="T18" s="51" t="s">
         <v>101</v>
       </c>
-      <c r="U18" s="54" t="s">
+      <c r="U18" s="49" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2518,8 +2552,8 @@
         <v>178</v>
       </c>
       <c r="E19" s="19"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="28" t="s">
+      <c r="F19" s="37"/>
+      <c r="G19" s="27" t="s">
         <v>129</v>
       </c>
       <c r="H19" s="5">
@@ -2528,7 +2562,7 @@
       <c r="I19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J19" s="45" t="s">
+      <c r="J19" s="42" t="s">
         <v>149</v>
       </c>
       <c r="K19" s="4" t="s">
@@ -2543,19 +2577,19 @@
       <c r="P19" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Q19" s="53">
+      <c r="Q19" s="48">
         <v>9</v>
       </c>
-      <c r="R19" s="54" t="s">
+      <c r="R19" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="S19" s="53" t="s">
+      <c r="S19" s="48" t="s">
         <v>126</v>
       </c>
-      <c r="T19" s="56" t="s">
+      <c r="T19" s="51" t="s">
         <v>129</v>
       </c>
-      <c r="U19" s="54" t="s">
+      <c r="U19" s="49" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2573,44 +2607,44 @@
         <v>178</v>
       </c>
       <c r="E20" s="22"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="28" t="s">
+      <c r="F20" s="38"/>
+      <c r="G20" s="95" t="s">
         <v>102</v>
       </c>
-      <c r="H20" s="5">
+      <c r="H20" s="88">
         <v>18</v>
       </c>
-      <c r="I20" s="3" t="s">
+      <c r="I20" s="89" t="s">
         <v>20</v>
       </c>
-      <c r="J20" s="20" t="s">
+      <c r="J20" s="96" t="s">
         <v>150</v>
       </c>
-      <c r="K20" s="4" t="s">
+      <c r="K20" s="89" t="s">
         <v>19</v>
       </c>
-      <c r="L20" s="12" t="s">
+      <c r="L20" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="M20" s="21"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="23"/>
-      <c r="P20" s="7" t="s">
+      <c r="M20" s="87"/>
+      <c r="N20" s="91"/>
+      <c r="O20" s="95"/>
+      <c r="P20" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="Q20" s="53">
+      <c r="Q20" s="48">
         <v>9</v>
       </c>
-      <c r="R20" s="54" t="s">
+      <c r="R20" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="S20" s="53" t="s">
+      <c r="S20" s="48" t="s">
         <v>126</v>
       </c>
-      <c r="T20" s="56" t="s">
+      <c r="T20" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="U20" s="54" t="s">
+      <c r="U20" s="49" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2628,44 +2662,44 @@
         <v>178</v>
       </c>
       <c r="E21" s="17"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="28" t="s">
+      <c r="F21" s="39"/>
+      <c r="G21" s="95" t="s">
         <v>103</v>
       </c>
-      <c r="H21" s="5">
+      <c r="H21" s="88">
         <v>19</v>
       </c>
-      <c r="I21" s="3" t="s">
+      <c r="I21" s="89" t="s">
         <v>20</v>
       </c>
-      <c r="J21" s="24" t="s">
+      <c r="J21" s="101" t="s">
         <v>151</v>
       </c>
-      <c r="K21" s="9" t="s">
+      <c r="K21" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="L21" s="12" t="s">
+      <c r="L21" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="M21" s="21"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="23"/>
-      <c r="P21" s="47" t="s">
+      <c r="M21" s="87"/>
+      <c r="N21" s="91"/>
+      <c r="O21" s="95"/>
+      <c r="P21" s="102" t="s">
         <v>20</v>
       </c>
-      <c r="Q21" s="53">
+      <c r="Q21" s="48">
         <v>9</v>
       </c>
-      <c r="R21" s="54" t="s">
+      <c r="R21" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="S21" s="53" t="s">
+      <c r="S21" s="48" t="s">
         <v>126</v>
       </c>
-      <c r="T21" s="56" t="s">
+      <c r="T21" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="U21" s="54" t="s">
+      <c r="U21" s="49" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2683,8 +2717,8 @@
         <v>178</v>
       </c>
       <c r="E22" s="22"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="28" t="s">
+      <c r="F22" s="38"/>
+      <c r="G22" s="27" t="s">
         <v>134</v>
       </c>
       <c r="H22" s="5">
@@ -2693,7 +2727,7 @@
       <c r="I22" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="27" t="s">
+      <c r="J22" s="26" t="s">
         <v>175</v>
       </c>
       <c r="K22" s="9" t="s">
@@ -2712,19 +2746,19 @@
       <c r="P22" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Q22" s="57">
+      <c r="Q22" s="52">
         <v>6</v>
       </c>
-      <c r="R22" s="54" t="s">
+      <c r="R22" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="S22" s="57" t="s">
+      <c r="S22" s="52" t="s">
         <v>89</v>
       </c>
-      <c r="T22" s="58" t="s">
+      <c r="T22" s="53" t="s">
         <v>166</v>
       </c>
-      <c r="U22" s="59" t="s">
+      <c r="U22" s="54" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2744,8 +2778,8 @@
       <c r="E23" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="F23" s="41"/>
-      <c r="G23" s="28" t="s">
+      <c r="F23" s="38"/>
+      <c r="G23" s="27" t="s">
         <v>176</v>
       </c>
       <c r="H23" s="5">
@@ -2754,7 +2788,7 @@
       <c r="I23" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J23" s="27" t="s">
+      <c r="J23" s="26" t="s">
         <v>177</v>
       </c>
       <c r="K23" s="9" t="s">
@@ -2773,19 +2807,19 @@
       <c r="P23" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Q23" s="53">
+      <c r="Q23" s="48">
         <v>6</v>
       </c>
-      <c r="R23" s="54" t="s">
+      <c r="R23" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="S23" s="53" t="s">
+      <c r="S23" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="T23" s="55" t="s">
+      <c r="T23" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="U23" s="54" t="s">
+      <c r="U23" s="49" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2802,8 +2836,8 @@
       <c r="D24" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="F24" s="41"/>
-      <c r="G24" s="28" t="s">
+      <c r="F24" s="38"/>
+      <c r="G24" s="27" t="s">
         <v>108</v>
       </c>
       <c r="H24" s="5">
@@ -2812,7 +2846,7 @@
       <c r="I24" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J24" s="46" t="s">
+      <c r="J24" s="43" t="s">
         <v>152</v>
       </c>
       <c r="K24" s="4" t="s">
@@ -2827,19 +2861,19 @@
       <c r="P24" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Q24" s="53">
+      <c r="Q24" s="48">
         <v>9</v>
       </c>
-      <c r="R24" s="54" t="s">
+      <c r="R24" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="S24" s="53" t="s">
+      <c r="S24" s="48" t="s">
         <v>126</v>
       </c>
-      <c r="T24" s="56" t="s">
+      <c r="T24" s="51" t="s">
         <v>108</v>
       </c>
-      <c r="U24" s="54" t="s">
+      <c r="U24" s="49" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2856,48 +2890,48 @@
       <c r="D25" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="F25" s="41"/>
-      <c r="G25" s="28" t="s">
+      <c r="F25" s="38"/>
+      <c r="G25" s="95" t="s">
         <v>109</v>
       </c>
-      <c r="H25" s="5">
+      <c r="H25" s="88">
         <v>23</v>
       </c>
-      <c r="I25" s="3" t="s">
+      <c r="I25" s="89" t="s">
         <v>20</v>
       </c>
-      <c r="J25" s="20" t="s">
+      <c r="J25" s="96" t="s">
         <v>153</v>
       </c>
-      <c r="K25" s="4" t="s">
+      <c r="K25" s="89" t="s">
         <v>19</v>
       </c>
-      <c r="L25" s="12" t="s">
+      <c r="L25" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="M25" s="13"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="23"/>
-      <c r="P25" s="7" t="s">
+      <c r="M25" s="91"/>
+      <c r="N25" s="91"/>
+      <c r="O25" s="95"/>
+      <c r="P25" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="Q25" s="53">
+      <c r="Q25" s="48">
         <v>9</v>
       </c>
-      <c r="R25" s="54" t="s">
+      <c r="R25" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="S25" s="53" t="s">
+      <c r="S25" s="48" t="s">
         <v>126</v>
       </c>
-      <c r="T25" s="56" t="s">
+      <c r="T25" s="51" t="s">
         <v>109</v>
       </c>
-      <c r="U25" s="54" t="s">
+      <c r="U25" s="49" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="26" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>110</v>
       </c>
@@ -2911,8 +2945,8 @@
         <v>87</v>
       </c>
       <c r="E26" s="22"/>
-      <c r="F26" s="41"/>
-      <c r="G26" s="28" t="s">
+      <c r="F26" s="38"/>
+      <c r="G26" s="27" t="s">
         <v>136</v>
       </c>
       <c r="H26" s="5">
@@ -2921,7 +2955,7 @@
       <c r="I26" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="46" t="s">
+      <c r="J26" s="43" t="s">
         <v>179</v>
       </c>
       <c r="K26" s="4" t="s">
@@ -2936,11 +2970,11 @@
       <c r="P26" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Q26" s="60"/>
-      <c r="R26" s="61"/>
-      <c r="S26" s="60"/>
-      <c r="T26" s="62"/>
-      <c r="U26" s="61"/>
+      <c r="Q26" s="55"/>
+      <c r="R26" s="56"/>
+      <c r="S26" s="55"/>
+      <c r="T26" s="57"/>
+      <c r="U26" s="56"/>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
@@ -2956,8 +2990,8 @@
         <v>87</v>
       </c>
       <c r="E27" s="22"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="28" t="s">
+      <c r="F27" s="38"/>
+      <c r="G27" s="27" t="s">
         <v>137</v>
       </c>
       <c r="H27" s="5">
@@ -2981,23 +3015,23 @@
       <c r="P27" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Q27" s="53">
+      <c r="Q27" s="48">
         <v>9</v>
       </c>
-      <c r="R27" s="54" t="s">
+      <c r="R27" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="S27" s="53" t="s">
+      <c r="S27" s="48" t="s">
         <v>126</v>
       </c>
-      <c r="T27" s="56" t="s">
+      <c r="T27" s="51" t="s">
         <v>137</v>
       </c>
-      <c r="U27" s="54" t="s">
+      <c r="U27" s="49" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="28" spans="1:21" s="35" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>110</v>
       </c>
@@ -3011,49 +3045,57 @@
         <v>170</v>
       </c>
       <c r="E28" s="22"/>
-      <c r="F28" s="41"/>
-      <c r="G28" s="28" t="s">
+      <c r="F28" s="38"/>
+      <c r="G28" s="95" t="s">
         <v>138</v>
       </c>
-      <c r="H28" s="5">
+      <c r="H28" s="88">
         <v>26</v>
       </c>
-      <c r="I28" s="3" t="s">
+      <c r="I28" s="89" t="s">
         <v>20</v>
       </c>
-      <c r="J28" s="46" t="s">
+      <c r="J28" s="103" t="s">
         <v>143</v>
       </c>
-      <c r="K28" s="4" t="s">
+      <c r="K28" s="89" t="s">
         <v>19</v>
       </c>
-      <c r="L28" s="12" t="s">
+      <c r="L28" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="M28" s="13"/>
-      <c r="N28" s="13"/>
-      <c r="O28" s="23"/>
-      <c r="P28" s="7" t="s">
+      <c r="M28" s="91"/>
+      <c r="N28" s="91"/>
+      <c r="O28" s="95"/>
+      <c r="P28" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="Q28" s="53">
+      <c r="Q28" s="48">
         <v>9</v>
       </c>
-      <c r="R28" s="54" t="s">
+      <c r="R28" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="S28" s="53" t="s">
+      <c r="S28" s="48" t="s">
         <v>126</v>
       </c>
-      <c r="T28" s="56" t="s">
+      <c r="T28" s="51" t="s">
         <v>104</v>
       </c>
-      <c r="U28" s="54" t="s">
+      <c r="U28" s="49" t="s">
         <v>128</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:S2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -3066,14 +3108,6 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="S1:S2"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P3">

</xml_diff>

<commit_message>
Escaleta mat 10 tema 2
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado10/guion02/ESCALETA_MA_10_02_CO.xlsx
+++ b/fuentes/contenidos/grado10/guion02/ESCALETA_MA_10_02_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EdgarJosué\Documents\GitHub\Matematicas\fuentes\contenidos\grado10\guion02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado10\guion02\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="180">
   <si>
     <t>Asignatura</t>
   </si>
@@ -370,13 +370,7 @@
     <t>No</t>
   </si>
   <si>
-    <t>2° ESO</t>
-  </si>
-  <si>
     <t>Los ángulos</t>
-  </si>
-  <si>
-    <t>Banco de actividades: Los ángulos</t>
   </si>
   <si>
     <t>MT_08_06</t>
@@ -567,6 +561,9 @@
   </si>
   <si>
     <t>Los ángulos y los triángulos</t>
+  </si>
+  <si>
+    <t>¿Qué sabes de los ángulos?</t>
   </si>
 </sst>
 </file>
@@ -1056,15 +1053,6 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1075,93 +1063,6 @@
     <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1211,6 +1112,96 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1518,7 +1509,7 @@
   <dimension ref="A1:U28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+      <selection activeCell="X19" sqref="X19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1537,94 +1528,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="64" t="s">
+      <c r="C1" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="60" t="s">
+      <c r="D1" s="84" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="62" t="s">
+      <c r="E1" s="86" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="67" t="s">
+      <c r="F1" s="91" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="58" t="s">
+      <c r="G1" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="69" t="s">
+      <c r="H1" s="93" t="s">
         <v>78</v>
       </c>
-      <c r="I1" s="71" t="s">
+      <c r="I1" s="95" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="73" t="s">
+      <c r="J1" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="75" t="s">
+      <c r="K1" s="99" t="s">
         <v>73</v>
       </c>
-      <c r="L1" s="58" t="s">
+      <c r="L1" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="79" t="s">
+      <c r="M1" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="79"/>
-      <c r="O1" s="80" t="s">
+      <c r="N1" s="74"/>
+      <c r="O1" s="75" t="s">
         <v>74</v>
       </c>
-      <c r="P1" s="82" t="s">
+      <c r="P1" s="77" t="s">
         <v>79</v>
       </c>
-      <c r="Q1" s="84" t="s">
+      <c r="Q1" s="79" t="s">
         <v>65</v>
       </c>
-      <c r="R1" s="85" t="s">
+      <c r="R1" s="80" t="s">
         <v>66</v>
       </c>
-      <c r="S1" s="86" t="s">
+      <c r="S1" s="81" t="s">
         <v>67</v>
       </c>
-      <c r="T1" s="77" t="s">
+      <c r="T1" s="72" t="s">
         <v>68</v>
       </c>
-      <c r="U1" s="78" t="s">
+      <c r="U1" s="73" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="61"/>
-      <c r="B2" s="63"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="59"/>
+      <c r="A2" s="85"/>
+      <c r="B2" s="87"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="94"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="100"/>
+      <c r="L2" s="83"/>
       <c r="M2" s="44" t="s">
         <v>70</v>
       </c>
       <c r="N2" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="O2" s="81"/>
-      <c r="P2" s="83"/>
-      <c r="Q2" s="84"/>
-      <c r="R2" s="85"/>
-      <c r="S2" s="86"/>
-      <c r="T2" s="77"/>
-      <c r="U2" s="78"/>
+      <c r="O2" s="76"/>
+      <c r="P2" s="78"/>
+      <c r="Q2" s="79"/>
+      <c r="R2" s="80"/>
+      <c r="S2" s="81"/>
+      <c r="T2" s="72"/>
+      <c r="U2" s="73"/>
     </row>
     <row r="3" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -1634,53 +1625,53 @@
         <v>99</v>
       </c>
       <c r="C3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E3" s="34"/>
       <c r="F3" s="36"/>
-      <c r="G3" s="87" t="s">
+      <c r="G3" s="55" t="s">
         <v>111</v>
       </c>
-      <c r="H3" s="88">
+      <c r="H3" s="56">
         <v>1</v>
       </c>
-      <c r="I3" s="89" t="s">
+      <c r="I3" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="90" t="s">
+      <c r="J3" s="58" t="s">
         <v>112</v>
       </c>
-      <c r="K3" s="89" t="s">
+      <c r="K3" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="91" t="s">
+      <c r="L3" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="91"/>
-      <c r="N3" s="92"/>
-      <c r="O3" s="93" t="s">
+      <c r="M3" s="59"/>
+      <c r="N3" s="60"/>
+      <c r="O3" s="61" t="s">
         <v>113</v>
       </c>
-      <c r="P3" s="94" t="s">
+      <c r="P3" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="Q3" s="45" t="s">
+      <c r="Q3" s="102">
+        <v>8</v>
+      </c>
+      <c r="R3" s="101" t="s">
+        <v>98</v>
+      </c>
+      <c r="S3" s="102" t="s">
         <v>115</v>
       </c>
-      <c r="R3" s="46" t="s">
-        <v>98</v>
-      </c>
-      <c r="S3" s="45" t="s">
+      <c r="T3" s="103" t="s">
+        <v>179</v>
+      </c>
+      <c r="U3" s="101" t="s">
         <v>116</v>
-      </c>
-      <c r="T3" s="47" t="s">
-        <v>117</v>
-      </c>
-      <c r="U3" s="46" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -1691,15 +1682,15 @@
         <v>99</v>
       </c>
       <c r="C4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E4" s="34"/>
       <c r="F4" s="35"/>
       <c r="G4" s="41" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H4" s="5">
         <v>2</v>
@@ -1708,7 +1699,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="24" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>20</v>
@@ -1721,24 +1712,24 @@
         <v>33</v>
       </c>
       <c r="O4" s="30" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="P4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Q4" s="48">
+      <c r="Q4" s="45">
         <v>6</v>
       </c>
-      <c r="R4" s="49" t="s">
+      <c r="R4" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="S4" s="48" t="s">
+      <c r="S4" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="T4" s="50" t="s">
-        <v>164</v>
-      </c>
-      <c r="U4" s="49" t="s">
+      <c r="T4" s="47" t="s">
+        <v>162</v>
+      </c>
+      <c r="U4" s="46" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1750,15 +1741,15 @@
         <v>99</v>
       </c>
       <c r="C5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E5" s="34"/>
       <c r="F5" s="35"/>
       <c r="G5" s="40" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H5" s="5">
         <v>3</v>
@@ -1767,7 +1758,7 @@
         <v>20</v>
       </c>
       <c r="J5" s="28" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>20</v>
@@ -1780,24 +1771,24 @@
         <v>33</v>
       </c>
       <c r="O5" s="30" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="P5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Q5" s="48">
+      <c r="Q5" s="45">
         <v>6</v>
       </c>
-      <c r="R5" s="49" t="s">
+      <c r="R5" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="S5" s="48" t="s">
+      <c r="S5" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="T5" s="50" t="s">
+      <c r="T5" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="U5" s="49" t="s">
+      <c r="U5" s="46" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1809,15 +1800,15 @@
         <v>99</v>
       </c>
       <c r="C6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E6" s="34"/>
       <c r="F6" s="35"/>
       <c r="G6" s="40" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H6" s="5">
         <v>4</v>
@@ -1826,7 +1817,7 @@
         <v>20</v>
       </c>
       <c r="J6" s="28" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>20</v>
@@ -1840,19 +1831,19 @@
       <c r="P6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Q6" s="48">
+      <c r="Q6" s="45">
         <v>6</v>
       </c>
-      <c r="R6" s="49" t="s">
+      <c r="R6" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="S6" s="48" t="s">
+      <c r="S6" s="45" t="s">
         <v>92</v>
       </c>
-      <c r="T6" s="50" t="s">
-        <v>167</v>
-      </c>
-      <c r="U6" s="49" t="s">
+      <c r="T6" s="47" t="s">
+        <v>165</v>
+      </c>
+      <c r="U6" s="46" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1864,15 +1855,15 @@
         <v>99</v>
       </c>
       <c r="C7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E7" s="34"/>
       <c r="F7" s="35"/>
       <c r="G7" s="40" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H7" s="5">
         <v>5</v>
@@ -1881,7 +1872,7 @@
         <v>20</v>
       </c>
       <c r="J7" s="28" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>20</v>
@@ -1894,24 +1885,24 @@
         <v>32</v>
       </c>
       <c r="O7" s="30" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="P7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Q7" s="48">
+      <c r="Q7" s="45">
         <v>6</v>
       </c>
-      <c r="R7" s="49" t="s">
+      <c r="R7" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="S7" s="48" t="s">
+      <c r="S7" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="T7" s="50" t="s">
+      <c r="T7" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="U7" s="49" t="s">
+      <c r="U7" s="46" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1923,13 +1914,13 @@
         <v>99</v>
       </c>
       <c r="C8" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F8" s="37"/>
       <c r="G8" s="27" t="s">
@@ -1942,7 +1933,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="20" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K8" s="4" t="s">
         <v>19</v>
@@ -1956,20 +1947,20 @@
       <c r="P8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Q8" s="48">
+      <c r="Q8" s="45">
         <v>9</v>
       </c>
-      <c r="R8" s="49" t="s">
+      <c r="R8" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="S8" s="48" t="s">
+      <c r="S8" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="T8" s="48" t="s">
+        <v>105</v>
+      </c>
+      <c r="U8" s="46" t="s">
         <v>126</v>
-      </c>
-      <c r="T8" s="51" t="s">
-        <v>105</v>
-      </c>
-      <c r="U8" s="49" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -1980,7 +1971,7 @@
         <v>99</v>
       </c>
       <c r="C9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>100</v>
@@ -1988,7 +1979,7 @@
       <c r="E9" s="22"/>
       <c r="F9" s="38"/>
       <c r="G9" s="27" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H9" s="5">
         <v>7</v>
@@ -1997,7 +1988,7 @@
         <v>19</v>
       </c>
       <c r="J9" s="42" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>19</v>
@@ -2011,20 +2002,20 @@
       <c r="P9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Q9" s="48">
+      <c r="Q9" s="45">
         <v>9</v>
       </c>
-      <c r="R9" s="49" t="s">
+      <c r="R9" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="S9" s="48" t="s">
+      <c r="S9" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="T9" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="U9" s="46" t="s">
         <v>126</v>
-      </c>
-      <c r="T9" s="51" t="s">
-        <v>132</v>
-      </c>
-      <c r="U9" s="49" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -2035,7 +2026,7 @@
         <v>99</v>
       </c>
       <c r="C10" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D10" s="18" t="s">
         <v>100</v>
@@ -2043,7 +2034,7 @@
       <c r="E10" s="19"/>
       <c r="F10" s="37"/>
       <c r="G10" s="27" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H10" s="5">
         <v>8</v>
@@ -2052,7 +2043,7 @@
         <v>20</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="K10" s="4" t="s">
         <v>19</v>
@@ -2066,20 +2057,20 @@
       <c r="P10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Q10" s="48">
+      <c r="Q10" s="45">
         <v>9</v>
       </c>
-      <c r="R10" s="49" t="s">
+      <c r="R10" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="S10" s="48" t="s">
+      <c r="S10" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="T10" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="U10" s="46" t="s">
         <v>126</v>
-      </c>
-      <c r="T10" s="51" t="s">
-        <v>127</v>
-      </c>
-      <c r="U10" s="49" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -2090,7 +2081,7 @@
         <v>99</v>
       </c>
       <c r="C11" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D11" s="18" t="s">
         <v>100</v>
@@ -2098,7 +2089,7 @@
       <c r="E11" s="19"/>
       <c r="F11" s="37"/>
       <c r="G11" s="27" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H11" s="5">
         <v>9</v>
@@ -2107,7 +2098,7 @@
         <v>20</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K11" s="4" t="s">
         <v>20</v>
@@ -2120,24 +2111,24 @@
         <v>23</v>
       </c>
       <c r="O11" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="P11" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="48">
+      <c r="Q11" s="45">
         <v>6</v>
       </c>
-      <c r="R11" s="49" t="s">
+      <c r="R11" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="S11" s="48" t="s">
+      <c r="S11" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="T11" s="50" t="s">
-        <v>165</v>
-      </c>
-      <c r="U11" s="49" t="s">
+      <c r="T11" s="47" t="s">
+        <v>163</v>
+      </c>
+      <c r="U11" s="46" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2149,13 +2140,13 @@
         <v>99</v>
       </c>
       <c r="C12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D12" s="18" t="s">
         <v>100</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F12" s="31"/>
       <c r="G12" s="27" t="s">
@@ -2168,7 +2159,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="24" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K12" s="4" t="s">
         <v>19</v>
@@ -2182,20 +2173,20 @@
       <c r="P12" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Q12" s="48">
+      <c r="Q12" s="45">
         <v>9</v>
       </c>
-      <c r="R12" s="49" t="s">
+      <c r="R12" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="S12" s="48" t="s">
+      <c r="S12" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="T12" s="48" t="s">
+        <v>106</v>
+      </c>
+      <c r="U12" s="46" t="s">
         <v>126</v>
-      </c>
-      <c r="T12" s="51" t="s">
-        <v>106</v>
-      </c>
-      <c r="U12" s="49" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
@@ -2206,51 +2197,51 @@
         <v>99</v>
       </c>
       <c r="C13" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E13" s="22"/>
       <c r="F13" s="38"/>
-      <c r="G13" s="95" t="s">
-        <v>130</v>
-      </c>
-      <c r="H13" s="88">
+      <c r="G13" s="63" t="s">
+        <v>128</v>
+      </c>
+      <c r="H13" s="56">
         <v>11</v>
       </c>
-      <c r="I13" s="89" t="s">
+      <c r="I13" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="96" t="s">
-        <v>144</v>
-      </c>
-      <c r="K13" s="97" t="s">
+      <c r="J13" s="64" t="s">
+        <v>142</v>
+      </c>
+      <c r="K13" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="L13" s="91" t="s">
+      <c r="L13" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="M13" s="98"/>
-      <c r="N13" s="98"/>
-      <c r="O13" s="95"/>
-      <c r="P13" s="99" t="s">
+      <c r="M13" s="66"/>
+      <c r="N13" s="66"/>
+      <c r="O13" s="63"/>
+      <c r="P13" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="Q13" s="48">
+      <c r="Q13" s="45">
         <v>9</v>
       </c>
-      <c r="R13" s="49" t="s">
+      <c r="R13" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="S13" s="48" t="s">
+      <c r="S13" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="T13" s="48" t="s">
+        <v>128</v>
+      </c>
+      <c r="U13" s="46" t="s">
         <v>126</v>
-      </c>
-      <c r="T13" s="51" t="s">
-        <v>130</v>
-      </c>
-      <c r="U13" s="49" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -2261,54 +2252,54 @@
         <v>99</v>
       </c>
       <c r="C14" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E14" s="22"/>
       <c r="F14" s="38"/>
-      <c r="G14" s="95" t="s">
-        <v>173</v>
-      </c>
-      <c r="H14" s="88">
+      <c r="G14" s="63" t="s">
+        <v>171</v>
+      </c>
+      <c r="H14" s="56">
         <v>12</v>
       </c>
-      <c r="I14" s="89" t="s">
+      <c r="I14" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="96" t="s">
-        <v>145</v>
-      </c>
-      <c r="K14" s="97" t="s">
+      <c r="J14" s="64" t="s">
+        <v>143</v>
+      </c>
+      <c r="K14" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="91" t="s">
+      <c r="L14" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="M14" s="87"/>
-      <c r="N14" s="91" t="s">
+      <c r="M14" s="55"/>
+      <c r="N14" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="O14" s="95" t="s">
-        <v>161</v>
-      </c>
-      <c r="P14" s="99" t="s">
+      <c r="O14" s="63" t="s">
+        <v>159</v>
+      </c>
+      <c r="P14" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="Q14" s="48">
+      <c r="Q14" s="45">
         <v>6</v>
       </c>
-      <c r="R14" s="49" t="s">
+      <c r="R14" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="S14" s="48" t="s">
+      <c r="S14" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="T14" s="50" t="s">
+      <c r="T14" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="U14" s="49" t="s">
+      <c r="U14" s="46" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2320,51 +2311,51 @@
         <v>99</v>
       </c>
       <c r="C15" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E15" s="22"/>
       <c r="F15" s="38"/>
-      <c r="G15" s="95" t="s">
-        <v>131</v>
-      </c>
-      <c r="H15" s="88">
+      <c r="G15" s="63" t="s">
+        <v>129</v>
+      </c>
+      <c r="H15" s="56">
         <v>13</v>
       </c>
-      <c r="I15" s="89" t="s">
+      <c r="I15" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="J15" s="100" t="s">
-        <v>146</v>
-      </c>
-      <c r="K15" s="97" t="s">
+      <c r="J15" s="68" t="s">
+        <v>144</v>
+      </c>
+      <c r="K15" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="L15" s="91" t="s">
+      <c r="L15" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="M15" s="91"/>
-      <c r="N15" s="91"/>
-      <c r="O15" s="95"/>
-      <c r="P15" s="99" t="s">
+      <c r="M15" s="59"/>
+      <c r="N15" s="59"/>
+      <c r="O15" s="63"/>
+      <c r="P15" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="Q15" s="48">
+      <c r="Q15" s="45">
         <v>9</v>
       </c>
-      <c r="R15" s="49" t="s">
+      <c r="R15" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="S15" s="48" t="s">
+      <c r="S15" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="T15" s="48" t="s">
+        <v>129</v>
+      </c>
+      <c r="U15" s="46" t="s">
         <v>126</v>
-      </c>
-      <c r="T15" s="51" t="s">
-        <v>131</v>
-      </c>
-      <c r="U15" s="49" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
@@ -2375,10 +2366,10 @@
         <v>99</v>
       </c>
       <c r="C16" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E16" s="22" t="s">
         <v>85</v>
@@ -2394,7 +2385,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="20" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="K16" s="4" t="s">
         <v>19</v>
@@ -2408,20 +2399,20 @@
       <c r="P16" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Q16" s="48">
+      <c r="Q16" s="45">
         <v>9</v>
       </c>
-      <c r="R16" s="49" t="s">
+      <c r="R16" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="S16" s="48" t="s">
+      <c r="S16" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="T16" s="48" t="s">
+        <v>107</v>
+      </c>
+      <c r="U16" s="46" t="s">
         <v>126</v>
-      </c>
-      <c r="T16" s="51" t="s">
-        <v>107</v>
-      </c>
-      <c r="U16" s="49" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
@@ -2432,54 +2423,54 @@
         <v>99</v>
       </c>
       <c r="C17" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E17" s="22"/>
       <c r="F17" s="38"/>
-      <c r="G17" s="95" t="s">
-        <v>135</v>
-      </c>
-      <c r="H17" s="88">
+      <c r="G17" s="63" t="s">
+        <v>133</v>
+      </c>
+      <c r="H17" s="56">
         <v>15</v>
       </c>
-      <c r="I17" s="89" t="s">
+      <c r="I17" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="96" t="s">
-        <v>174</v>
-      </c>
-      <c r="K17" s="89" t="s">
+      <c r="J17" s="64" t="s">
+        <v>172</v>
+      </c>
+      <c r="K17" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="L17" s="91" t="s">
+      <c r="L17" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="M17" s="91"/>
-      <c r="N17" s="91" t="s">
+      <c r="M17" s="59"/>
+      <c r="N17" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="O17" s="95" t="s">
-        <v>162</v>
-      </c>
-      <c r="P17" s="99" t="s">
+      <c r="O17" s="63" t="s">
+        <v>160</v>
+      </c>
+      <c r="P17" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="Q17" s="48">
+      <c r="Q17" s="45">
         <v>6</v>
       </c>
-      <c r="R17" s="49" t="s">
+      <c r="R17" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="S17" s="48" t="s">
+      <c r="S17" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="T17" s="50" t="s">
+      <c r="T17" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="U17" s="49" t="s">
+      <c r="U17" s="46" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2491,10 +2482,10 @@
         <v>99</v>
       </c>
       <c r="C18" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E18" s="19"/>
       <c r="F18" s="37"/>
@@ -2508,7 +2499,7 @@
         <v>20</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="K18" s="4" t="s">
         <v>19</v>
@@ -2522,20 +2513,20 @@
       <c r="P18" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Q18" s="48">
+      <c r="Q18" s="45">
         <v>9</v>
       </c>
-      <c r="R18" s="49" t="s">
+      <c r="R18" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="S18" s="48" t="s">
+      <c r="S18" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="T18" s="48" t="s">
+        <v>101</v>
+      </c>
+      <c r="U18" s="46" t="s">
         <v>126</v>
-      </c>
-      <c r="T18" s="51" t="s">
-        <v>101</v>
-      </c>
-      <c r="U18" s="49" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
@@ -2546,15 +2537,15 @@
         <v>99</v>
       </c>
       <c r="C19" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E19" s="19"/>
       <c r="F19" s="37"/>
       <c r="G19" s="27" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H19" s="5">
         <v>17</v>
@@ -2563,7 +2554,7 @@
         <v>19</v>
       </c>
       <c r="J19" s="42" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="K19" s="4" t="s">
         <v>19</v>
@@ -2577,20 +2568,20 @@
       <c r="P19" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Q19" s="48">
+      <c r="Q19" s="45">
         <v>9</v>
       </c>
-      <c r="R19" s="49" t="s">
+      <c r="R19" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="S19" s="48" t="s">
+      <c r="S19" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="T19" s="48" t="s">
+        <v>127</v>
+      </c>
+      <c r="U19" s="46" t="s">
         <v>126</v>
-      </c>
-      <c r="T19" s="51" t="s">
-        <v>129</v>
-      </c>
-      <c r="U19" s="49" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
@@ -2601,51 +2592,51 @@
         <v>99</v>
       </c>
       <c r="C20" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E20" s="22"/>
       <c r="F20" s="38"/>
-      <c r="G20" s="95" t="s">
+      <c r="G20" s="63" t="s">
         <v>102</v>
       </c>
-      <c r="H20" s="88">
+      <c r="H20" s="56">
         <v>18</v>
       </c>
-      <c r="I20" s="89" t="s">
+      <c r="I20" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="J20" s="96" t="s">
-        <v>150</v>
-      </c>
-      <c r="K20" s="89" t="s">
+      <c r="J20" s="64" t="s">
+        <v>148</v>
+      </c>
+      <c r="K20" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="L20" s="91" t="s">
+      <c r="L20" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="M20" s="87"/>
-      <c r="N20" s="91"/>
-      <c r="O20" s="95"/>
-      <c r="P20" s="99" t="s">
+      <c r="M20" s="55"/>
+      <c r="N20" s="59"/>
+      <c r="O20" s="63"/>
+      <c r="P20" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="Q20" s="48">
+      <c r="Q20" s="45">
         <v>9</v>
       </c>
-      <c r="R20" s="49" t="s">
+      <c r="R20" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="S20" s="48" t="s">
+      <c r="S20" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="T20" s="48" t="s">
+        <v>102</v>
+      </c>
+      <c r="U20" s="46" t="s">
         <v>126</v>
-      </c>
-      <c r="T20" s="51" t="s">
-        <v>102</v>
-      </c>
-      <c r="U20" s="49" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
@@ -2656,51 +2647,51 @@
         <v>99</v>
       </c>
       <c r="C21" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="39"/>
-      <c r="G21" s="95" t="s">
+      <c r="G21" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="H21" s="88">
+      <c r="H21" s="56">
         <v>19</v>
       </c>
-      <c r="I21" s="89" t="s">
+      <c r="I21" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="J21" s="101" t="s">
-        <v>151</v>
-      </c>
-      <c r="K21" s="97" t="s">
+      <c r="J21" s="69" t="s">
+        <v>149</v>
+      </c>
+      <c r="K21" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="L21" s="91" t="s">
+      <c r="L21" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="M21" s="87"/>
-      <c r="N21" s="91"/>
-      <c r="O21" s="95"/>
-      <c r="P21" s="102" t="s">
+      <c r="M21" s="55"/>
+      <c r="N21" s="59"/>
+      <c r="O21" s="63"/>
+      <c r="P21" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="Q21" s="48">
+      <c r="Q21" s="45">
         <v>9</v>
       </c>
-      <c r="R21" s="49" t="s">
+      <c r="R21" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="S21" s="48" t="s">
+      <c r="S21" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="T21" s="48" t="s">
+        <v>103</v>
+      </c>
+      <c r="U21" s="46" t="s">
         <v>126</v>
-      </c>
-      <c r="T21" s="51" t="s">
-        <v>103</v>
-      </c>
-      <c r="U21" s="49" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
@@ -2711,15 +2702,15 @@
         <v>99</v>
       </c>
       <c r="C22" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E22" s="22"/>
       <c r="F22" s="38"/>
       <c r="G22" s="27" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H22" s="5">
         <v>20</v>
@@ -2728,7 +2719,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="26" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K22" s="9" t="s">
         <v>20</v>
@@ -2741,24 +2732,24 @@
         <v>48</v>
       </c>
       <c r="O22" s="23" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="P22" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Q22" s="52">
+      <c r="Q22" s="49">
         <v>6</v>
       </c>
-      <c r="R22" s="49" t="s">
+      <c r="R22" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="S22" s="52" t="s">
+      <c r="S22" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="T22" s="53" t="s">
-        <v>166</v>
-      </c>
-      <c r="U22" s="54" t="s">
+      <c r="T22" s="50" t="s">
+        <v>164</v>
+      </c>
+      <c r="U22" s="51" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2770,17 +2761,17 @@
         <v>99</v>
       </c>
       <c r="C23" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E23" s="22" t="s">
         <v>85</v>
       </c>
       <c r="F23" s="38"/>
       <c r="G23" s="27" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H23" s="5">
         <v>21</v>
@@ -2789,7 +2780,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="26" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="K23" s="9" t="s">
         <v>20</v>
@@ -2802,24 +2793,24 @@
         <v>84</v>
       </c>
       <c r="O23" s="23" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="P23" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Q23" s="48">
+      <c r="Q23" s="45">
         <v>6</v>
       </c>
-      <c r="R23" s="49" t="s">
+      <c r="R23" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="S23" s="48" t="s">
+      <c r="S23" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="T23" s="50" t="s">
+      <c r="T23" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="U23" s="49" t="s">
+      <c r="U23" s="46" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2831,7 +2822,7 @@
         <v>99</v>
       </c>
       <c r="C24" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D24" s="22" t="s">
         <v>86</v>
@@ -2847,7 +2838,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="43" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="K24" s="4" t="s">
         <v>19</v>
@@ -2861,20 +2852,20 @@
       <c r="P24" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Q24" s="48">
+      <c r="Q24" s="45">
         <v>9</v>
       </c>
-      <c r="R24" s="49" t="s">
+      <c r="R24" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="S24" s="48" t="s">
+      <c r="S24" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="T24" s="48" t="s">
+        <v>108</v>
+      </c>
+      <c r="U24" s="46" t="s">
         <v>126</v>
-      </c>
-      <c r="T24" s="51" t="s">
-        <v>108</v>
-      </c>
-      <c r="U24" s="49" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
@@ -2885,50 +2876,50 @@
         <v>99</v>
       </c>
       <c r="C25" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D25" s="22" t="s">
         <v>86</v>
       </c>
       <c r="F25" s="38"/>
-      <c r="G25" s="95" t="s">
+      <c r="G25" s="63" t="s">
         <v>109</v>
       </c>
-      <c r="H25" s="88">
+      <c r="H25" s="56">
         <v>23</v>
       </c>
-      <c r="I25" s="89" t="s">
+      <c r="I25" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="J25" s="96" t="s">
-        <v>153</v>
-      </c>
-      <c r="K25" s="89" t="s">
+      <c r="J25" s="64" t="s">
+        <v>151</v>
+      </c>
+      <c r="K25" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="L25" s="91" t="s">
+      <c r="L25" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="M25" s="91"/>
-      <c r="N25" s="91"/>
-      <c r="O25" s="95"/>
-      <c r="P25" s="99" t="s">
+      <c r="M25" s="59"/>
+      <c r="N25" s="59"/>
+      <c r="O25" s="63"/>
+      <c r="P25" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="Q25" s="48">
+      <c r="Q25" s="45">
         <v>9</v>
       </c>
-      <c r="R25" s="49" t="s">
+      <c r="R25" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="S25" s="48" t="s">
+      <c r="S25" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="T25" s="48" t="s">
+        <v>109</v>
+      </c>
+      <c r="U25" s="46" t="s">
         <v>126</v>
-      </c>
-      <c r="T25" s="51" t="s">
-        <v>109</v>
-      </c>
-      <c r="U25" s="49" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:21" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -2939,7 +2930,7 @@
         <v>99</v>
       </c>
       <c r="C26" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>87</v>
@@ -2947,7 +2938,7 @@
       <c r="E26" s="22"/>
       <c r="F26" s="38"/>
       <c r="G26" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H26" s="5">
         <v>24</v>
@@ -2956,7 +2947,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="43" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K26" s="4" t="s">
         <v>20</v>
@@ -2970,11 +2961,11 @@
       <c r="P26" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Q26" s="55"/>
-      <c r="R26" s="56"/>
-      <c r="S26" s="55"/>
-      <c r="T26" s="57"/>
-      <c r="U26" s="56"/>
+      <c r="Q26" s="52"/>
+      <c r="R26" s="53"/>
+      <c r="S26" s="52"/>
+      <c r="T26" s="54"/>
+      <c r="U26" s="53"/>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
@@ -2984,7 +2975,7 @@
         <v>99</v>
       </c>
       <c r="C27" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D27" s="18" t="s">
         <v>87</v>
@@ -2992,7 +2983,7 @@
       <c r="E27" s="22"/>
       <c r="F27" s="38"/>
       <c r="G27" s="27" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H27" s="5">
         <v>25</v>
@@ -3001,7 +2992,7 @@
         <v>20</v>
       </c>
       <c r="J27" s="20" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="K27" s="4" t="s">
         <v>20</v>
@@ -3015,20 +3006,20 @@
       <c r="P27" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="Q27" s="48">
+      <c r="Q27" s="45">
         <v>9</v>
       </c>
-      <c r="R27" s="49" t="s">
+      <c r="R27" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="S27" s="48" t="s">
+      <c r="S27" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="T27" s="48" t="s">
+        <v>135</v>
+      </c>
+      <c r="U27" s="46" t="s">
         <v>126</v>
-      </c>
-      <c r="T27" s="51" t="s">
-        <v>137</v>
-      </c>
-      <c r="U27" s="49" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="28" spans="1:21" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -3039,63 +3030,55 @@
         <v>99</v>
       </c>
       <c r="C28" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E28" s="22"/>
       <c r="F28" s="38"/>
-      <c r="G28" s="95" t="s">
-        <v>138</v>
-      </c>
-      <c r="H28" s="88">
+      <c r="G28" s="63" t="s">
+        <v>136</v>
+      </c>
+      <c r="H28" s="56">
         <v>26</v>
       </c>
-      <c r="I28" s="89" t="s">
+      <c r="I28" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="J28" s="103" t="s">
-        <v>143</v>
-      </c>
-      <c r="K28" s="89" t="s">
+      <c r="J28" s="71" t="s">
+        <v>141</v>
+      </c>
+      <c r="K28" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="L28" s="91" t="s">
+      <c r="L28" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="M28" s="91"/>
-      <c r="N28" s="91"/>
-      <c r="O28" s="95"/>
-      <c r="P28" s="99" t="s">
+      <c r="M28" s="59"/>
+      <c r="N28" s="59"/>
+      <c r="O28" s="63"/>
+      <c r="P28" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="Q28" s="48">
+      <c r="Q28" s="45">
         <v>9</v>
       </c>
-      <c r="R28" s="49" t="s">
+      <c r="R28" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="S28" s="48" t="s">
+      <c r="S28" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="T28" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="U28" s="46" t="s">
         <v>126</v>
-      </c>
-      <c r="T28" s="51" t="s">
-        <v>104</v>
-      </c>
-      <c r="U28" s="49" t="s">
-        <v>128</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="S1:S2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -3108,6 +3091,14 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:S2"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P3">

</xml_diff>